<commit_message>
Code draft before refactoring
</commit_message>
<xml_diff>
--- a/resources/Score_Validierung.xlsx
+++ b/resources/Score_Validierung.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilanorup/Desktop/Studium/MSc/MA/Score_Validierung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gilanorup/Desktop/Studium/MSc/MA/code/masters_thesis_gn/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D216CF-8312-3D47-A558-EC1A94A244AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66938EFC-8045-7749-BD71-C3DB491D81F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="500" windowWidth="24980" windowHeight="19700" xr2:uid="{AA4B4F69-C3B5-D24B-AA52-CB6A8FF10934}"/>
+    <workbookView xWindow="9380" yWindow="740" windowWidth="19300" windowHeight="17140" activeTab="2" xr2:uid="{AA4B4F69-C3B5-D24B-AA52-CB6A8FF10934}"/>
   </bookViews>
   <sheets>
     <sheet name="scores_manuell" sheetId="1" r:id="rId1"/>
     <sheet name="language_task_scores" sheetId="2" r:id="rId2"/>
+    <sheet name="bias" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,10 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
-  <si>
-    <t>subject_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="241">
   <si>
     <t>semantic_fluency_score</t>
   </si>
@@ -655,13 +653,121 @@
   </si>
   <si>
     <t>ostrich,penguin,queenbee,zebra,walrus</t>
+  </si>
+  <si>
+    <t>Subject_ID</t>
+  </si>
+  <si>
+    <t>picture_naming_score_a</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mouth organ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">african accent </t>
+  </si>
+  <si>
+    <t xml:space="preserve">is actually usa, wrote ENGLISH_AMERICAN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mouth accordeon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mouth organ, audio qualität nicht so gut </t>
+  </si>
+  <si>
+    <t xml:space="preserve">background noise (TV or radio), hangmans noose </t>
+  </si>
+  <si>
+    <t xml:space="preserve">spontaneous speech tasks sehr elaborate &amp; varied language (on first glance) </t>
+  </si>
+  <si>
+    <t>sugar tong, canoo, rhinosaurus, abokus, theodolite stand / artists easel</t>
+  </si>
+  <si>
+    <t>mouth organ, sugar tongs, nose, abecus</t>
+  </si>
+  <si>
+    <t>trypod, apecus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nicht soo elaborate </t>
+  </si>
+  <si>
+    <t>mouth organ or harmonica, sugar tweezers, cano, rino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dromady, ice tongs, brinocerus, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">einfachere Beschreibungen </t>
+  </si>
+  <si>
+    <t>ice tongs</t>
+  </si>
+  <si>
+    <t>tweezers, aber auch cano</t>
+  </si>
+  <si>
+    <t>mouth organ -&gt; harmonica, sugar tongs, swings</t>
+  </si>
+  <si>
+    <t>interesting descriptions "all the people have one mouth, one nose, two eyes and probably two eyebrows."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accent; mouth orgon, dominose, rainocerus, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">einfachere, kürzere Beschreibungen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">anuse, </t>
+  </si>
+  <si>
+    <t>apicus, cano -&gt; spielt also keine Rolle</t>
+  </si>
+  <si>
+    <t>elaborate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sehr detaillierte Beschreibungen (viel Text) </t>
+  </si>
+  <si>
+    <t>wenig Beschreibungen</t>
+  </si>
+  <si>
+    <t>nicht so viele Beschreibungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">viele Beschreibungen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tongs, harmonica </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -672,6 +778,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -696,9 +808,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1035,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{396283D2-0ACE-1B47-96E9-96B235EAF910}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1055,28 +1168,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1087,22 +1200,22 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1">
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="1">
         <v>20</v>
@@ -1116,22 +1229,22 @@
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1">
         <v>19</v>
@@ -1145,22 +1258,22 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>23</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1">
         <v>17</v>
@@ -1174,22 +1287,22 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="G5" s="1">
         <v>12</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="1">
         <v>20</v>
@@ -1203,22 +1316,22 @@
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="G6" s="1">
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="1">
         <v>16</v>
@@ -1232,22 +1345,22 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="G7" s="1">
         <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="1">
         <v>19</v>
@@ -1261,22 +1374,22 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="G8" s="1">
         <v>23</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="1">
         <v>18</v>
@@ -1290,22 +1403,22 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1">
         <v>22</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="1">
         <v>18</v>
@@ -1319,22 +1432,22 @@
         <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="G10" s="1">
         <v>26</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I10" s="1">
         <v>17</v>
@@ -1348,22 +1461,22 @@
         <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="I11" s="1">
         <v>18</v>
@@ -1377,22 +1490,22 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="I12" s="1">
         <v>19</v>
@@ -1406,22 +1519,22 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G13" s="1">
         <v>19</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I13" s="1">
         <v>20</v>
@@ -1435,22 +1548,22 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G14" s="1">
         <v>23</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I14" s="1">
         <v>19</v>
@@ -1464,19 +1577,19 @@
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="G15" s="1">
         <v>22</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I15" s="1">
         <v>17</v>
@@ -1490,22 +1603,22 @@
         <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="G16" s="1">
-        <v>19</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="I16" s="1">
         <v>18</v>
@@ -1519,22 +1632,22 @@
         <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G17" s="1">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I17" s="1">
         <v>17</v>
@@ -1548,22 +1661,22 @@
         <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="G18" s="1">
         <v>4</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I18" s="1">
         <v>9</v>
@@ -1577,22 +1690,22 @@
         <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="G19" s="1">
         <v>11</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I19" s="1">
         <v>10</v>
@@ -1606,19 +1719,19 @@
         <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="G20" s="1">
         <v>11</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I20" s="1">
         <v>20</v>
@@ -1632,22 +1745,22 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="1">
+        <v>18</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21" s="1">
-        <v>18</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="I21" s="1">
         <v>19</v>
@@ -1661,22 +1774,22 @@
         <v>18</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" s="1">
-        <v>17</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="I22" s="1">
         <v>18</v>
@@ -1690,22 +1803,22 @@
         <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="G23" s="1">
-        <v>17</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="I23" s="1">
         <v>20</v>
@@ -1719,16 +1832,16 @@
         <v>8</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="G24" s="1">
         <v>14</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I24" s="1">
         <v>8</v>
@@ -1742,22 +1855,22 @@
         <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="G25" s="1">
         <v>21</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I25" s="1">
         <v>18</v>
@@ -1771,22 +1884,22 @@
         <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1">
+        <v>20</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="G26" s="1">
-        <v>20</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="I26" s="1">
         <v>19</v>
@@ -1800,19 +1913,19 @@
         <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="G27" s="1">
         <v>13</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I27" s="1">
         <v>19</v>
@@ -1826,22 +1939,22 @@
         <v>16</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="G28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="I28" s="1">
         <v>20</v>
@@ -1855,22 +1968,22 @@
         <v>13</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="G29" s="1">
         <v>14</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I29" s="1">
         <v>15</v>
@@ -1884,22 +1997,22 @@
         <v>15</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="G30" s="1">
         <v>13</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I30" s="1">
         <v>20</v>
@@ -1913,22 +2026,22 @@
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="G31" s="1">
         <v>14</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I31" s="1">
         <v>15</v>
@@ -1942,22 +2055,22 @@
         <v>21</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="G32" s="1">
         <v>22</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I32" s="1">
         <v>16</v>
@@ -1971,22 +2084,22 @@
         <v>22</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="G33" s="1">
         <v>12</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I33" s="1">
         <v>19</v>
@@ -2000,22 +2113,22 @@
         <v>23</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1">
+        <v>15</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" s="1">
-        <v>15</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="I34" s="1">
         <v>15</v>
@@ -2029,19 +2142,19 @@
         <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="G35" s="1">
         <v>11</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I35" s="1">
         <v>18</v>
@@ -2055,22 +2168,22 @@
         <v>22</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="G36" s="1">
         <v>13</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I36" s="1">
         <v>20</v>
@@ -2084,22 +2197,22 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1">
+        <v>19</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="G37" s="1">
-        <v>19</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="I37" s="1">
         <v>18</v>
@@ -2113,22 +2226,22 @@
         <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="G38" s="1">
         <v>25</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I38" s="1">
         <v>17</v>
@@ -2142,22 +2255,22 @@
         <v>22</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1">
+        <v>16</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="G39" s="1">
-        <v>16</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="I39" s="1">
         <v>20</v>
@@ -2171,22 +2284,22 @@
         <v>19</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="G40" s="1">
         <v>4</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I40" s="1">
         <v>20</v>
@@ -2200,22 +2313,22 @@
         <v>19</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1">
+        <v>18</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="G41" s="1">
-        <v>18</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="I41" s="1">
         <v>19</v>
@@ -2235,7 +2348,7 @@
   <dimension ref="A1:D1004"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F1" sqref="F1:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2245,16 +2358,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -16257,4 +16370,848 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F858BE20-9CB0-2048-89B9-3633BD636E40}">
+  <dimension ref="A1:G45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="58.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>275</v>
+      </c>
+      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>300</v>
+      </c>
+      <c r="B3" s="2">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>321</v>
+      </c>
+      <c r="B4" s="2">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>348</v>
+      </c>
+      <c r="B5" s="2">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>361</v>
+      </c>
+      <c r="B6" s="2">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>401</v>
+      </c>
+      <c r="B7" s="2">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G7" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>434</v>
+      </c>
+      <c r="B8" s="2">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>448</v>
+      </c>
+      <c r="B9" s="2">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>17</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E9" t="s">
+        <v>211</v>
+      </c>
+      <c r="F9" t="s">
+        <v>228</v>
+      </c>
+      <c r="G9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>468</v>
+      </c>
+      <c r="B10" s="2">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>494</v>
+      </c>
+      <c r="B11" s="2">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>516</v>
+      </c>
+      <c r="B12" s="2">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E12" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>574</v>
+      </c>
+      <c r="B13" s="2">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" t="s">
+        <v>210</v>
+      </c>
+      <c r="F13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>584</v>
+      </c>
+      <c r="B14" s="2">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E14" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" t="s">
+        <v>213</v>
+      </c>
+      <c r="G14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>649</v>
+      </c>
+      <c r="B15" s="2">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>676</v>
+      </c>
+      <c r="B16" s="2">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>737</v>
+      </c>
+      <c r="B17" s="2">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>750</v>
+      </c>
+      <c r="B18" s="2">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E18" t="s">
+        <v>210</v>
+      </c>
+      <c r="F18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>802</v>
+      </c>
+      <c r="B19" s="2">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E19" t="s">
+        <v>211</v>
+      </c>
+      <c r="F19" t="s">
+        <v>233</v>
+      </c>
+      <c r="G19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>842</v>
+      </c>
+      <c r="B20" s="2">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F20" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>857</v>
+      </c>
+      <c r="B21" s="2">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>19</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>889</v>
+      </c>
+      <c r="B22" s="2">
+        <v>18</v>
+      </c>
+      <c r="C22">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E22" t="s">
+        <v>210</v>
+      </c>
+      <c r="G22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>934</v>
+      </c>
+      <c r="B23" s="2">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E23" t="s">
+        <v>210</v>
+      </c>
+      <c r="F23" t="s">
+        <v>215</v>
+      </c>
+      <c r="G23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>952</v>
+      </c>
+      <c r="B24" s="2">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>7</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E24" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>971</v>
+      </c>
+      <c r="B25" s="2">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E25" t="s">
+        <v>211</v>
+      </c>
+      <c r="G25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>991</v>
+      </c>
+      <c r="B26" s="2">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E26" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>1005</v>
+      </c>
+      <c r="B27" s="2">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>1025</v>
+      </c>
+      <c r="B28" s="2">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E28" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>1027</v>
+      </c>
+      <c r="B29" s="2">
+        <v>15</v>
+      </c>
+      <c r="C29">
+        <v>14</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E29" t="s">
+        <v>211</v>
+      </c>
+      <c r="G29" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>1044</v>
+      </c>
+      <c r="B30" s="2">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E30" t="s">
+        <v>210</v>
+      </c>
+      <c r="F30" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>1060</v>
+      </c>
+      <c r="B31" s="2">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>1080</v>
+      </c>
+      <c r="B32" s="2">
+        <v>16</v>
+      </c>
+      <c r="C32">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>1101</v>
+      </c>
+      <c r="B33" s="2">
+        <v>19</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E33" t="s">
+        <v>210</v>
+      </c>
+      <c r="F33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>1104</v>
+      </c>
+      <c r="B34" s="2">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E34" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>1128</v>
+      </c>
+      <c r="B35" s="2">
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <v>18</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" t="s">
+        <v>210</v>
+      </c>
+      <c r="G35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>1175</v>
+      </c>
+      <c r="B36" s="2">
+        <v>20</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E36" t="s">
+        <v>211</v>
+      </c>
+      <c r="G36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>1186</v>
+      </c>
+      <c r="B37" s="2">
+        <v>18</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E37" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>1192</v>
+      </c>
+      <c r="B38" s="2">
+        <v>17</v>
+      </c>
+      <c r="C38">
+        <v>17</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E38" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>1196</v>
+      </c>
+      <c r="B39" s="2">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>19</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>1249</v>
+      </c>
+      <c r="B40" s="2">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>20</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>1295</v>
+      </c>
+      <c r="B41" s="2">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" t="s">
+        <v>210</v>
+      </c>
+      <c r="G41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <f>COUNTIF(D2:D41, "uk")</f>
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <f>COUNTIF(E2:E41, "m")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D45">
+        <f>COUNTIF(D2:D42, "usa")</f>
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <f>COUNTIF(E2:E41, "f")</f>
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>